<commit_message>
Ver producto especifico agregado
</commit_message>
<xml_diff>
--- a/Files/ElSaborJose.xlsx
+++ b/Files/ElSaborJose.xlsx
@@ -639,7 +639,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Helado</t>
+          <t>helado</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -653,22 +653,10 @@
       <c r="A11" t="n">
         <v>10</v>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Postres</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Helado</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>2</v>
-      </c>
-      <c r="E11" t="n">
-        <v>13</v>
-      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">

</xml_diff>